<commit_message>
lente contato inicio 1.1.9
</commit_message>
<xml_diff>
--- a/views/financeiro/relatorios/resumo_campanha_67.xlsx
+++ b/views/financeiro/relatorios/resumo_campanha_67.xlsx
@@ -718,19 +718,19 @@
         <v>19</v>
       </c>
       <c r="C11" s="6">
+        <v>1950.0</v>
+      </c>
+      <c r="D11" s="6">
         <v>600.0</v>
       </c>
-      <c r="D11" s="6">
-        <v>0</v>
-      </c>
       <c r="E11" s="6">
-        <v>600.0</v>
+        <v>1350.0</v>
       </c>
       <c r="F11" s="7">
-        <v>1.0</v>
+        <v>0.69230769230769</v>
       </c>
       <c r="G11" s="6">
-        <v>6.0</v>
+        <v>13.5</v>
       </c>
       <c r="H11" s="8">
         <v>0</v>
@@ -744,19 +744,19 @@
         <v>20</v>
       </c>
       <c r="C12" s="6">
-        <v>5650.0</v>
+        <v>6000.0</v>
       </c>
       <c r="D12" s="6">
         <v>4900.0</v>
       </c>
       <c r="E12" s="6">
-        <v>750.0</v>
+        <v>1100.0</v>
       </c>
       <c r="F12" s="7">
-        <v>0.13274336283186</v>
+        <v>0.18333333333333</v>
       </c>
       <c r="G12" s="6">
-        <v>7.5</v>
+        <v>11.0</v>
       </c>
       <c r="H12" s="8">
         <v>0</v>
@@ -770,19 +770,19 @@
         <v>21</v>
       </c>
       <c r="C13" s="9">
-        <v>13128.0</v>
+        <v>14828.0</v>
       </c>
       <c r="D13" s="9">
-        <v>9000.0</v>
+        <v>9600.0</v>
       </c>
       <c r="E13" s="9">
-        <v>4128.0</v>
+        <v>5228.0</v>
       </c>
       <c r="F13" s="10">
-        <v>0.31444241316271</v>
+        <v>0.35257620717561</v>
       </c>
       <c r="G13" s="9">
-        <v>41.28</v>
+        <v>52.28</v>
       </c>
       <c r="H13" s="9">
         <v>0</v>
@@ -967,19 +967,19 @@
         <v>27</v>
       </c>
       <c r="C24" s="6">
-        <v>13128.0</v>
+        <v>14828.0</v>
       </c>
       <c r="D24" s="6">
-        <v>9000.0</v>
+        <v>9600.0</v>
       </c>
       <c r="E24" s="6">
-        <v>4128.0</v>
+        <v>5228.0</v>
       </c>
       <c r="F24" s="7">
-        <v>0.31444241316271</v>
+        <v>0.35257620717561</v>
       </c>
       <c r="G24" s="6">
-        <v>41.28</v>
+        <v>52.28</v>
       </c>
       <c r="H24" s="8">
         <v>0</v>
@@ -1045,19 +1045,19 @@
         <v>21</v>
       </c>
       <c r="C27" s="9">
-        <v>16268.0</v>
+        <v>17968.0</v>
       </c>
       <c r="D27" s="9">
-        <v>10490.0</v>
+        <v>11090.0</v>
       </c>
       <c r="E27" s="9">
-        <v>5778.0</v>
+        <v>6878.0</v>
       </c>
       <c r="F27" s="10">
-        <v>0.35517580526186</v>
+        <v>0.38279162956367</v>
       </c>
       <c r="G27" s="9">
-        <v>57.78</v>
+        <v>68.78</v>
       </c>
       <c r="H27" s="9">
         <v>0</v>
@@ -1147,13 +1147,13 @@
         <v>19</v>
       </c>
       <c r="D34" s="12">
+        <v>1950.0</v>
+      </c>
+      <c r="E34" s="13">
         <v>600.0</v>
       </c>
-      <c r="E34" s="13">
-        <v>0</v>
-      </c>
       <c r="F34" s="12">
-        <v>600.0</v>
+        <v>1350.0</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -1164,13 +1164,13 @@
         <v>20</v>
       </c>
       <c r="D35" s="12">
-        <v>5650.0</v>
+        <v>6000.0</v>
       </c>
       <c r="E35" s="13">
         <v>4900.0</v>
       </c>
       <c r="F35" s="12">
-        <v>750.0</v>
+        <v>1100.0</v>
       </c>
     </row>
     <row r="36" spans="1:9">
@@ -1211,15 +1211,15 @@
       </c>
       <c r="D39" s="9">
         <f>sum(D31:D38)</f>
-        <v>16268</v>
+        <v>17968</v>
       </c>
       <c r="E39" s="9">
         <f>sum(E31:E38)</f>
-        <v>10490</v>
+        <v>11090</v>
       </c>
       <c r="F39" s="9">
         <f>sum(F31:F38)</f>
-        <v>5778</v>
+        <v>6878</v>
       </c>
     </row>
     <row r="40" spans="1:9">
@@ -1228,7 +1228,7 @@
       </c>
       <c r="E40" s="15">
         <f>(E39/D39)</f>
-        <v>0.64482419473814</v>
+        <v>0.61720837043633</v>
       </c>
     </row>
     <row r="41" spans="1:9">
@@ -1237,7 +1237,7 @@
       </c>
       <c r="E41" s="15">
         <f>(F39/D39)</f>
-        <v>0.35517580526186</v>
+        <v>0.38279162956367</v>
       </c>
     </row>
   </sheetData>

</xml_diff>